<commit_message>
Code and JavaDoc Cleanup
- moved the expanded part from MctseChanceNode and MctseExpecNode to MctseNode
</commit_message>
<xml_diff>
--- a/agents/EWN/3x3 2 Players G-0/csv/mode1-EWN3x3-EEXPAND-false.xlsx
+++ b/agents/EWN/3x3 2 Players G-0/csv/mode1-EWN3x3-EEXPAND-false.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20379"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wolfgang\Documents\GitHub\GBG\agents\EWN\3x3 2 Players G-0\csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A1B32962-570D-4795-BAD4-B25CC294DA8E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73CFB349-CCCF-4B29-A250-BEAC43A43DF6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8592"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8592" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mode1-EWN3x3-EEXPAND-false" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -896,11 +896,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32:H38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2067,6 +2067,12 @@
         <v>0</v>
       </c>
     </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I40">
+        <f>SUM(I4:I39)</f>
+        <v>444.71199999999993</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>